<commit_message>
ANR for elec and h2 production data
</commit_message>
<xml_diff>
--- a/Python/Data/NewPlantData/NewTechFramework.xlsx
+++ b/Python/Data/NewPlantData/NewTechFramework.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atpha\Documents\Postdocs\Projects\BlueToZeroH2\Model\Python\Data\NewPlantData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\Blue-to-Zero-H2\Python\Data\NewPlantData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63C1772-AEE5-47A0-9398-FCEF2E007C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD8AF93-BA23-4D28-8810-7BC6234CE7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30615" yWindow="6495" windowWidth="16755" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewTechFramework" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="90">
   <si>
     <t>PlantType</t>
   </si>
@@ -254,6 +267,42 @@
   </si>
   <si>
     <t>h2_turbine</t>
+  </si>
+  <si>
+    <t>iMSR</t>
+  </si>
+  <si>
+    <t>ANRElec</t>
+  </si>
+  <si>
+    <t>iPWR</t>
+  </si>
+  <si>
+    <t>HTGR</t>
+  </si>
+  <si>
+    <t>Micro</t>
+  </si>
+  <si>
+    <t>ANRH2</t>
+  </si>
+  <si>
+    <t>PBRHTGR</t>
+  </si>
+  <si>
+    <t>iPWRHTSE</t>
+  </si>
+  <si>
+    <t>HTGRHTSE</t>
+  </si>
+  <si>
+    <t>PBRHTGRHTSE</t>
+  </si>
+  <si>
+    <t>iMSRHTSE</t>
+  </si>
+  <si>
+    <t>MicroHTSE</t>
   </si>
 </sst>
 </file>
@@ -1067,41 +1116,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X17"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B23" sqref="B23:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.265625" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1328125" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="9" width="8.59765625" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" customWidth="1"/>
+    <col min="11" max="11" width="6.73046875" customWidth="1"/>
+    <col min="12" max="12" width="4.19921875" customWidth="1"/>
+    <col min="13" max="13" width="9.19921875" customWidth="1"/>
+    <col min="14" max="14" width="6.9296875" customWidth="1"/>
+    <col min="15" max="15" width="6.73046875" customWidth="1"/>
+    <col min="16" max="16" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.1328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1224,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1237,7 +1286,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1299,7 +1348,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1361,7 +1410,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1423,7 +1472,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1485,7 +1534,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1547,7 +1596,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1612,7 +1661,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1677,7 +1726,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1744,7 +1793,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1808,7 +1857,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -1868,7 +1917,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -1924,7 +1973,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -1980,7 +2029,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -2042,7 +2091,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -2104,7 +2153,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -2164,6 +2213,461 @@
       </c>
       <c r="X17" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18">
+        <v>77</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>60</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>30</v>
+      </c>
+      <c r="R18" t="s">
+        <v>30</v>
+      </c>
+      <c r="S18" t="s">
+        <v>30</v>
+      </c>
+      <c r="T18" t="s">
+        <v>30</v>
+      </c>
+      <c r="U18" t="s">
+        <v>30</v>
+      </c>
+      <c r="V18" t="s">
+        <v>30</v>
+      </c>
+      <c r="W18" t="s">
+        <v>30</v>
+      </c>
+      <c r="X18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19">
+        <v>164</v>
+      </c>
+      <c r="K19" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>60</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>30</v>
+      </c>
+      <c r="R19" t="s">
+        <v>30</v>
+      </c>
+      <c r="S19" t="s">
+        <v>30</v>
+      </c>
+      <c r="T19" t="s">
+        <v>30</v>
+      </c>
+      <c r="U19" t="s">
+        <v>30</v>
+      </c>
+      <c r="V19" t="s">
+        <v>30</v>
+      </c>
+      <c r="W19" t="s">
+        <v>30</v>
+      </c>
+      <c r="X19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20">
+        <v>80</v>
+      </c>
+      <c r="K20" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>60</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>30</v>
+      </c>
+      <c r="R20" t="s">
+        <v>30</v>
+      </c>
+      <c r="S20" t="s">
+        <v>30</v>
+      </c>
+      <c r="T20" t="s">
+        <v>30</v>
+      </c>
+      <c r="U20" t="s">
+        <v>30</v>
+      </c>
+      <c r="V20" t="s">
+        <v>30</v>
+      </c>
+      <c r="W20" t="s">
+        <v>30</v>
+      </c>
+      <c r="X20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21">
+        <v>141</v>
+      </c>
+      <c r="K21" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>60</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>30</v>
+      </c>
+      <c r="R21" t="s">
+        <v>30</v>
+      </c>
+      <c r="S21" t="s">
+        <v>30</v>
+      </c>
+      <c r="T21" t="s">
+        <v>30</v>
+      </c>
+      <c r="U21" t="s">
+        <v>30</v>
+      </c>
+      <c r="V21" t="s">
+        <v>30</v>
+      </c>
+      <c r="W21" t="s">
+        <v>30</v>
+      </c>
+      <c r="X21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22">
+        <v>6.7</v>
+      </c>
+      <c r="K22" t="s">
+        <v>33</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>60</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>30</v>
+      </c>
+      <c r="R22" t="s">
+        <v>30</v>
+      </c>
+      <c r="S22" t="s">
+        <v>30</v>
+      </c>
+      <c r="T22" t="s">
+        <v>30</v>
+      </c>
+      <c r="U22" t="s">
+        <v>30</v>
+      </c>
+      <c r="V22" t="s">
+        <v>30</v>
+      </c>
+      <c r="W22" t="s">
+        <v>30</v>
+      </c>
+      <c r="X22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23">
+        <v>77</v>
+      </c>
+      <c r="G23">
+        <v>100</v>
+      </c>
+      <c r="K23" t="s">
+        <v>33</v>
+      </c>
+      <c r="X23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24">
+        <v>164</v>
+      </c>
+      <c r="G24">
+        <v>30</v>
+      </c>
+      <c r="K24" t="s">
+        <v>33</v>
+      </c>
+      <c r="X24" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B25" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25">
+        <v>80</v>
+      </c>
+      <c r="G25">
+        <v>10</v>
+      </c>
+      <c r="K25" t="s">
+        <v>33</v>
+      </c>
+      <c r="X25" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26">
+        <v>141</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>33</v>
+      </c>
+      <c r="X26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27">
+        <v>6.7</v>
+      </c>
+      <c r="G27">
+        <v>50</v>
+      </c>
+      <c r="K27" t="s">
+        <v>33</v>
+      </c>
+      <c r="X27" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ANR for electricity production to new technology dataset
</commit_message>
<xml_diff>
--- a/Python/Data/NewPlantData/NewTechFramework.xlsx
+++ b/Python/Data/NewPlantData/NewTechFramework.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atpha\Documents\Postdocs\Projects\BlueToZeroH2\Model\Python\Data\NewPlantData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\Blue-to-Zero-H2\Python\Data\NewPlantData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63C1772-AEE5-47A0-9398-FCEF2E007C56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C70A505-CD0E-4880-8A2B-661CA1DCD383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30615" yWindow="6495" windowWidth="16755" windowHeight="10380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewTechFramework" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="84">
   <si>
     <t>PlantType</t>
   </si>
@@ -254,6 +267,24 @@
   </si>
   <si>
     <t>h2_turbine</t>
+  </si>
+  <si>
+    <t>iPWR</t>
+  </si>
+  <si>
+    <t>HTGR</t>
+  </si>
+  <si>
+    <t>PBRHTGR</t>
+  </si>
+  <si>
+    <t>iMSR</t>
+  </si>
+  <si>
+    <t>Micro</t>
+  </si>
+  <si>
+    <t>ANRElec</t>
   </si>
 </sst>
 </file>
@@ -1067,41 +1098,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X17"/>
+  <dimension ref="A1:X22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X18" sqref="X18:X22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.3984375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="31.1328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1175,7 +1206,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1237,7 +1268,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1299,7 +1330,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -1361,7 +1392,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1423,7 +1454,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -1485,7 +1516,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1547,7 +1578,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1612,7 +1643,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1677,7 +1708,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1744,7 +1775,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1808,7 +1839,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -1868,7 +1899,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -1924,7 +1955,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>65</v>
       </c>
@@ -1980,7 +2011,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -2042,7 +2073,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -2104,7 +2135,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -2164,6 +2195,286 @@
       </c>
       <c r="X17" t="s">
         <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18">
+        <v>77</v>
+      </c>
+      <c r="K18" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>60</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>30</v>
+      </c>
+      <c r="R18" t="s">
+        <v>30</v>
+      </c>
+      <c r="S18" t="s">
+        <v>30</v>
+      </c>
+      <c r="U18" t="s">
+        <v>30</v>
+      </c>
+      <c r="V18" t="s">
+        <v>30</v>
+      </c>
+      <c r="W18" t="s">
+        <v>30</v>
+      </c>
+      <c r="X18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19">
+        <v>164</v>
+      </c>
+      <c r="K19" t="s">
+        <v>33</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>60</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>30</v>
+      </c>
+      <c r="R19" t="s">
+        <v>30</v>
+      </c>
+      <c r="S19" t="s">
+        <v>30</v>
+      </c>
+      <c r="U19" t="s">
+        <v>30</v>
+      </c>
+      <c r="V19" t="s">
+        <v>30</v>
+      </c>
+      <c r="W19" t="s">
+        <v>30</v>
+      </c>
+      <c r="X19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20">
+        <v>80</v>
+      </c>
+      <c r="K20" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>60</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>30</v>
+      </c>
+      <c r="R20" t="s">
+        <v>30</v>
+      </c>
+      <c r="S20" t="s">
+        <v>30</v>
+      </c>
+      <c r="U20" t="s">
+        <v>30</v>
+      </c>
+      <c r="V20" t="s">
+        <v>30</v>
+      </c>
+      <c r="W20" t="s">
+        <v>30</v>
+      </c>
+      <c r="X20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21">
+        <v>141</v>
+      </c>
+      <c r="K21" t="s">
+        <v>33</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>60</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>30</v>
+      </c>
+      <c r="R21" t="s">
+        <v>30</v>
+      </c>
+      <c r="S21" t="s">
+        <v>30</v>
+      </c>
+      <c r="U21" t="s">
+        <v>30</v>
+      </c>
+      <c r="V21" t="s">
+        <v>30</v>
+      </c>
+      <c r="W21" t="s">
+        <v>30</v>
+      </c>
+      <c r="X21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22">
+        <v>6.7</v>
+      </c>
+      <c r="K22" t="s">
+        <v>33</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>20</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>30</v>
+      </c>
+      <c r="R22" t="s">
+        <v>30</v>
+      </c>
+      <c r="S22" t="s">
+        <v>30</v>
+      </c>
+      <c r="U22" t="s">
+        <v>30</v>
+      </c>
+      <c r="V22" t="s">
+        <v>30</v>
+      </c>
+      <c r="W22" t="s">
+        <v>30</v>
+      </c>
+      <c r="X22" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data for new anr-h2 systems
</commit_message>
<xml_diff>
--- a/Python/Data/NewPlantData/NewTechFramework.xlsx
+++ b/Python/Data/NewPlantData/NewTechFramework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\Blue-to-Zero-H2\Python\Data\NewPlantData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C70A505-CD0E-4880-8A2B-661CA1DCD383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA91A64-0AB1-4F6F-A7DE-780321F331C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewTechFramework" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="90">
   <si>
     <t>PlantType</t>
   </si>
@@ -285,6 +285,24 @@
   </si>
   <si>
     <t>ANRElec</t>
+  </si>
+  <si>
+    <t>iPWRHTSE</t>
+  </si>
+  <si>
+    <t>HTGRHTSE</t>
+  </si>
+  <si>
+    <t>PBRHTGRHTSE</t>
+  </si>
+  <si>
+    <t>iMSRHTSE</t>
+  </si>
+  <si>
+    <t>MicroHTSE</t>
+  </si>
+  <si>
+    <t>ANRH2</t>
   </si>
 </sst>
 </file>
@@ -1098,10 +1116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18:X22"/>
+      <selection activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2477,6 +2495,286 @@
         <v>41</v>
       </c>
     </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23">
+        <v>77</v>
+      </c>
+      <c r="K23" t="s">
+        <v>33</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>60</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>30</v>
+      </c>
+      <c r="R23" t="s">
+        <v>30</v>
+      </c>
+      <c r="S23" t="s">
+        <v>30</v>
+      </c>
+      <c r="U23" t="s">
+        <v>30</v>
+      </c>
+      <c r="V23" t="s">
+        <v>30</v>
+      </c>
+      <c r="W23" t="s">
+        <v>30</v>
+      </c>
+      <c r="X23" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F24">
+        <v>164</v>
+      </c>
+      <c r="K24" t="s">
+        <v>33</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>60</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>30</v>
+      </c>
+      <c r="R24" t="s">
+        <v>30</v>
+      </c>
+      <c r="S24" t="s">
+        <v>30</v>
+      </c>
+      <c r="U24" t="s">
+        <v>30</v>
+      </c>
+      <c r="V24" t="s">
+        <v>30</v>
+      </c>
+      <c r="W24" t="s">
+        <v>30</v>
+      </c>
+      <c r="X24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>86</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F25">
+        <v>80</v>
+      </c>
+      <c r="K25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>60</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>30</v>
+      </c>
+      <c r="R25" t="s">
+        <v>30</v>
+      </c>
+      <c r="S25" t="s">
+        <v>30</v>
+      </c>
+      <c r="U25" t="s">
+        <v>30</v>
+      </c>
+      <c r="V25" t="s">
+        <v>30</v>
+      </c>
+      <c r="W25" t="s">
+        <v>30</v>
+      </c>
+      <c r="X25" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>87</v>
+      </c>
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+      <c r="F26">
+        <v>141</v>
+      </c>
+      <c r="K26" t="s">
+        <v>33</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>60</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>30</v>
+      </c>
+      <c r="R26" t="s">
+        <v>30</v>
+      </c>
+      <c r="S26" t="s">
+        <v>30</v>
+      </c>
+      <c r="U26" t="s">
+        <v>30</v>
+      </c>
+      <c r="V26" t="s">
+        <v>30</v>
+      </c>
+      <c r="W26" t="s">
+        <v>30</v>
+      </c>
+      <c r="X26" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27">
+        <v>6.7</v>
+      </c>
+      <c r="K27" t="s">
+        <v>33</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>20</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>30</v>
+      </c>
+      <c r="R27" t="s">
+        <v>30</v>
+      </c>
+      <c r="S27" t="s">
+        <v>30</v>
+      </c>
+      <c r="U27" t="s">
+        <v>30</v>
+      </c>
+      <c r="V27" t="s">
+        <v>30</v>
+      </c>
+      <c r="W27" t="s">
+        <v>30</v>
+      </c>
+      <c r="X27" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new plant data spreadsheets
</commit_message>
<xml_diff>
--- a/Python/Data/NewPlantData/NewTechFramework.xlsx
+++ b/Python/Data/NewPlantData/NewTechFramework.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgarrou\Projects\Blue-to-Zero-H2\Python\Data\NewPlantData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CA91A64-0AB1-4F6F-A7DE-780321F331C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FF345E-9421-4C7A-AA3E-7B6FD217A96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewTechFramework" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="78">
   <si>
     <t>PlantType</t>
   </si>
@@ -267,42 +267,6 @@
   </si>
   <si>
     <t>h2_turbine</t>
-  </si>
-  <si>
-    <t>iPWR</t>
-  </si>
-  <si>
-    <t>HTGR</t>
-  </si>
-  <si>
-    <t>PBRHTGR</t>
-  </si>
-  <si>
-    <t>iMSR</t>
-  </si>
-  <si>
-    <t>Micro</t>
-  </si>
-  <si>
-    <t>ANRElec</t>
-  </si>
-  <si>
-    <t>iPWRHTSE</t>
-  </si>
-  <si>
-    <t>HTGRHTSE</t>
-  </si>
-  <si>
-    <t>PBRHTGRHTSE</t>
-  </si>
-  <si>
-    <t>iMSRHTSE</t>
-  </si>
-  <si>
-    <t>MicroHTSE</t>
-  </si>
-  <si>
-    <t>ANRH2</t>
   </si>
 </sst>
 </file>
@@ -1116,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W31" sqref="W31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2215,566 +2179,6 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18">
-        <v>77</v>
-      </c>
-      <c r="K18" t="s">
-        <v>33</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>60</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>30</v>
-      </c>
-      <c r="R18" t="s">
-        <v>30</v>
-      </c>
-      <c r="S18" t="s">
-        <v>30</v>
-      </c>
-      <c r="U18" t="s">
-        <v>30</v>
-      </c>
-      <c r="V18" t="s">
-        <v>30</v>
-      </c>
-      <c r="W18" t="s">
-        <v>30</v>
-      </c>
-      <c r="X18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>83</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19">
-        <v>164</v>
-      </c>
-      <c r="K19" t="s">
-        <v>33</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>60</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>30</v>
-      </c>
-      <c r="R19" t="s">
-        <v>30</v>
-      </c>
-      <c r="S19" t="s">
-        <v>30</v>
-      </c>
-      <c r="U19" t="s">
-        <v>30</v>
-      </c>
-      <c r="V19" t="s">
-        <v>30</v>
-      </c>
-      <c r="W19" t="s">
-        <v>30</v>
-      </c>
-      <c r="X19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B20" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20">
-        <v>80</v>
-      </c>
-      <c r="K20" t="s">
-        <v>33</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>60</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>30</v>
-      </c>
-      <c r="R20" t="s">
-        <v>30</v>
-      </c>
-      <c r="S20" t="s">
-        <v>30</v>
-      </c>
-      <c r="U20" t="s">
-        <v>30</v>
-      </c>
-      <c r="V20" t="s">
-        <v>30</v>
-      </c>
-      <c r="W20" t="s">
-        <v>30</v>
-      </c>
-      <c r="X20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" t="s">
-        <v>83</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21">
-        <v>141</v>
-      </c>
-      <c r="K21" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-      <c r="M21">
-        <v>0</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21">
-        <v>60</v>
-      </c>
-      <c r="Q21" t="s">
-        <v>30</v>
-      </c>
-      <c r="R21" t="s">
-        <v>30</v>
-      </c>
-      <c r="S21" t="s">
-        <v>30</v>
-      </c>
-      <c r="U21" t="s">
-        <v>30</v>
-      </c>
-      <c r="V21" t="s">
-        <v>30</v>
-      </c>
-      <c r="W21" t="s">
-        <v>30</v>
-      </c>
-      <c r="X21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>82</v>
-      </c>
-      <c r="B22" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22">
-        <v>6.7</v>
-      </c>
-      <c r="K22" t="s">
-        <v>33</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22">
-        <v>0</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22">
-        <v>20</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>30</v>
-      </c>
-      <c r="R22" t="s">
-        <v>30</v>
-      </c>
-      <c r="S22" t="s">
-        <v>30</v>
-      </c>
-      <c r="U22" t="s">
-        <v>30</v>
-      </c>
-      <c r="V22" t="s">
-        <v>30</v>
-      </c>
-      <c r="W22" t="s">
-        <v>30</v>
-      </c>
-      <c r="X22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23">
-        <v>77</v>
-      </c>
-      <c r="K23" t="s">
-        <v>33</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>60</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>30</v>
-      </c>
-      <c r="R23" t="s">
-        <v>30</v>
-      </c>
-      <c r="S23" t="s">
-        <v>30</v>
-      </c>
-      <c r="U23" t="s">
-        <v>30</v>
-      </c>
-      <c r="V23" t="s">
-        <v>30</v>
-      </c>
-      <c r="W23" t="s">
-        <v>30</v>
-      </c>
-      <c r="X23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24">
-        <v>164</v>
-      </c>
-      <c r="K24" t="s">
-        <v>33</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-      <c r="M24">
-        <v>0</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24">
-        <v>60</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>30</v>
-      </c>
-      <c r="R24" t="s">
-        <v>30</v>
-      </c>
-      <c r="S24" t="s">
-        <v>30</v>
-      </c>
-      <c r="U24" t="s">
-        <v>30</v>
-      </c>
-      <c r="V24" t="s">
-        <v>30</v>
-      </c>
-      <c r="W24" t="s">
-        <v>30</v>
-      </c>
-      <c r="X24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>86</v>
-      </c>
-      <c r="B25" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" t="s">
-        <v>73</v>
-      </c>
-      <c r="F25">
-        <v>80</v>
-      </c>
-      <c r="K25" t="s">
-        <v>33</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25">
-        <v>60</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>30</v>
-      </c>
-      <c r="R25" t="s">
-        <v>30</v>
-      </c>
-      <c r="S25" t="s">
-        <v>30</v>
-      </c>
-      <c r="U25" t="s">
-        <v>30</v>
-      </c>
-      <c r="V25" t="s">
-        <v>30</v>
-      </c>
-      <c r="W25" t="s">
-        <v>30</v>
-      </c>
-      <c r="X25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" t="s">
-        <v>73</v>
-      </c>
-      <c r="F26">
-        <v>141</v>
-      </c>
-      <c r="K26" t="s">
-        <v>33</v>
-      </c>
-      <c r="L26">
-        <v>0</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>60</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>30</v>
-      </c>
-      <c r="R26" t="s">
-        <v>30</v>
-      </c>
-      <c r="S26" t="s">
-        <v>30</v>
-      </c>
-      <c r="U26" t="s">
-        <v>30</v>
-      </c>
-      <c r="V26" t="s">
-        <v>30</v>
-      </c>
-      <c r="W26" t="s">
-        <v>30</v>
-      </c>
-      <c r="X26" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>88</v>
-      </c>
-      <c r="B27" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E27" t="s">
-        <v>73</v>
-      </c>
-      <c r="F27">
-        <v>6.7</v>
-      </c>
-      <c r="K27" t="s">
-        <v>33</v>
-      </c>
-      <c r="L27">
-        <v>0</v>
-      </c>
-      <c r="M27">
-        <v>0</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27">
-        <v>20</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>30</v>
-      </c>
-      <c r="R27" t="s">
-        <v>30</v>
-      </c>
-      <c r="S27" t="s">
-        <v>30</v>
-      </c>
-      <c r="U27" t="s">
-        <v>30</v>
-      </c>
-      <c r="V27" t="s">
-        <v>30</v>
-      </c>
-      <c r="W27" t="s">
-        <v>30</v>
-      </c>
-      <c r="X27" t="s">
-        <v>89</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>